<commit_message>
Correccion en los Reports para no indicar motivos de rechazo incorrectos
</commit_message>
<xml_diff>
--- a/ComentariosSobreLotes/CORRECCIONES.xlsx
+++ b/ComentariosSobreLotes/CORRECCIONES.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43239F0E-E504-4B5D-A8BA-0CA08445A3EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703C03B8-FC9E-4242-B729-2098AF115E35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>CORRECCIONES</t>
   </si>
@@ -40,10 +40,25 @@
     <t>En el report 2, el PDF que se genera, en la parte superior donde pone 5%IS el valor que muestra es el 10% y no el 5%</t>
   </si>
   <si>
-    <t>Ver BBDD1</t>
-  </si>
-  <si>
-    <t>Sigue mostrando como motivo de RECHAZO del LOTE en error 14.1 y no debería ser motivo de rechazo, solo identificarlo</t>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>Lo he corregido modificando ReportController (fila 297 y explicacion en la fila 302)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fila 323 de ReportController, en validaciones NO SE MULTIPLICA el Average por %IS </t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Sigue mostrando como motivo de RECHAZO del LOTE EN EL REPORT 2 error 14.1 y no debería ser motivo de rechazo, solo identificarlo</t>
+  </si>
+  <si>
+    <t>Sigue mostrando como motivo de RECHAZO del LOTE EN EL REPORT 3 error 14.1 y no debería ser motivo de rechazo, solo identificarlo</t>
+  </si>
+  <si>
+    <t>Lo he corregido modificando ReportController (fila 415 y explicacion en la fila 418)</t>
   </si>
 </sst>
 </file>
@@ -79,16 +94,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -106,12 +133,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9270E698-7A87-487D-8A54-572139AA3579}" name="Tabla1" displayName="Tabla1" ref="A1:C5" totalsRowShown="0">
-  <autoFilter ref="A1:C5" xr:uid="{1F22EB0C-582D-498B-9748-2452C8216B06}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9270E698-7A87-487D-8A54-572139AA3579}" name="Tabla1" displayName="Tabla1" ref="A1:C6" totalsRowShown="0">
+  <autoFilter ref="A1:C6" xr:uid="{1F22EB0C-582D-498B-9748-2452C8216B06}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{23FF449C-238A-47EB-A301-18DD5F1E77D7}" name="CORRECCIONES" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{11DB1B84-7B81-4EF6-A393-7CBF0E5981F3}" name="CORREGIDO?"/>
-    <tableColumn id="3" xr3:uid="{B7459DE0-81A9-40F2-B1A2-6724BF6CBEDB}" name="COMENTARIOS"/>
+    <tableColumn id="1" xr3:uid="{23FF449C-238A-47EB-A301-18DD5F1E77D7}" name="CORRECCIONES" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{11DB1B84-7B81-4EF6-A393-7CBF0E5981F3}" name="CORREGIDO?" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{B7459DE0-81A9-40F2-B1A2-6724BF6CBEDB}" name="COMENTARIOS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -383,7 +410,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -408,27 +435,52 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="C6" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>